<commit_message>
Searching about timers - in progress
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO.SXM1\Documents\GitHub\INMOOV_project\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI - embedded track\INMOOV\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B45AB783-27FC-4D5C-AD78-79AED03E5977}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68" xr2:uid="{762BE0AD-0318-4D37-A3B8-FD35501A490E}"/>
+    <workbookView xWindow="720" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -150,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -834,11 +833,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE4CB1C-E474-4CD3-A10E-32926A0EA0C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +904,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="9"/>
@@ -1543,7 +1542,7 @@
     <mergeCell ref="A16:H16"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H17:H29 H2:H15" xr:uid="{A640E8AE-D8AD-4009-961A-38F728581410}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H17:H29 H2:H15">
       <formula1>"Asseigned,In progress,done,Revised"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
move one servo using PWM
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI - embedded track\INMOOV\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mina\embeded_systems\ES_ITI_intake_40\Software_engineering\Calculator_repo\Software-Engineering\INMOOV_project\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68"/>
+    <workbookView xWindow="1665" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -837,7 +837,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +991,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="1"/>

</xml_diff>

<commit_message>
Moving Servo with AVR: Adding Code and Documents
To Be Tested
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68"/>
+    <workbookView xWindow="2610" yWindow="570" windowWidth="13935" windowHeight="10245" tabRatio="68"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -837,7 +837,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +991,7 @@
         <v>14</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="1"/>

</xml_diff>

<commit_message>
Timer Task in progress  Signed-off-by: areejhelal <areej_helal@yahoo.com>
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO.SXM1\Documents\GitHub\INMOOV_project\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basma\OneDrive\Desktop\new\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3B9550-3A93-481C-8BE6-2F67502517A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="68" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="68"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -467,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -583,15 +582,6 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -612,6 +602,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -874,26 +876,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="15" customWidth="1"/>
-    <col min="4" max="5" width="17.5703125" style="15" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="30.7265625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" style="15" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" style="15" customWidth="1"/>
+    <col min="4" max="5" width="17.54296875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -926,7 +928,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="7"/>
     </row>
-    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>6</v>
       </c>
@@ -955,7 +957,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
@@ -965,7 +967,9 @@
       <c r="C3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="49">
+        <v>43865</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="16">
         <v>43866</v>
@@ -974,7 +978,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="I3" s="19"/>
       <c r="J3" s="20"/>
@@ -984,7 +988,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
@@ -1013,7 +1017,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1046,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
@@ -1071,7 +1075,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>10</v>
       </c>
@@ -1100,14 +1104,14 @@
       <c r="N7" s="1"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="40">
         <v>43865</v>
       </c>
       <c r="D8" s="22"/>
@@ -1129,63 +1133,63 @@
       <c r="N8" s="1"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="1:15" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="35" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="43">
+      <c r="C9" s="40">
         <v>43865</v>
       </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="16">
         <v>43866</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="47"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
-      <c r="O9" s="48"/>
-    </row>
-    <row r="10" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="44"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
+      <c r="O9" s="45"/>
+    </row>
+    <row r="10" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="43">
+      <c r="C10" s="40">
         <v>43865</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="16">
         <v>43866</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="46" t="s">
+      <c r="G10" s="42"/>
+      <c r="H10" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I10" s="47"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="48"/>
-    </row>
-    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="I10" s="44"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="45"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="31" t="s">
         <v>16</v>
       </c>
@@ -1218,7 +1222,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="28" x14ac:dyDescent="0.35">
       <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
@@ -1249,7 +1253,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="28" x14ac:dyDescent="0.35">
       <c r="A13" s="31" t="s">
         <v>16</v>
       </c>
@@ -1280,7 +1284,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="28" x14ac:dyDescent="0.35">
       <c r="A14" s="31" t="s">
         <v>16</v>
       </c>
@@ -1311,7 +1315,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
@@ -1342,7 +1346,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="31" t="s">
         <v>23</v>
       </c>
@@ -1373,7 +1377,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="31" t="s">
         <v>24</v>
       </c>
@@ -1402,7 +1406,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18" s="31" t="s">
         <v>25</v>
       </c>
@@ -1431,17 +1435,17 @@
       <c r="N18" s="1"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="41"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
       <c r="I19" s="20"/>
       <c r="J19" s="25"/>
       <c r="K19" s="1"/>
@@ -1450,7 +1454,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="29"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1467,7 +1471,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="29"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1484,7 +1488,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="21"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="29"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1501,7 +1505,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="29"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1518,7 +1522,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="29"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1535,7 +1539,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="21"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="29"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1552,7 +1556,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="29"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1569,7 +1573,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="21"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="29"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1586,7 +1590,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="21"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="29"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1603,7 +1607,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="21"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="29"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1620,7 +1624,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="21"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="29"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1637,7 +1641,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="21"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="29"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1654,7 +1658,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="34"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
@@ -1676,7 +1680,7 @@
     <mergeCell ref="A19:H19"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H32 H2:H18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H32 H2:H18">
       <formula1>"Asseigned,In progress,done,Revised"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Finished searching about timers task Signed-off-by: ahmedRefaat95 <ahmed.refaat.rashad@gmail.com>
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basma\OneDrive\Desktop\new\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITI - embedded track\INMOOV\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -153,12 +153,15 @@
   </si>
   <si>
     <t>buy 9g servo and battery</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -603,6 +606,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,9 +616,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -879,23 +882,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="15" customWidth="1"/>
-    <col min="3" max="3" width="20.54296875" style="15" customWidth="1"/>
-    <col min="4" max="5" width="17.54296875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="26.453125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="15"/>
+    <col min="1" max="1" width="30.7109375" style="35" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="15" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="15" customWidth="1"/>
+    <col min="4" max="5" width="17.5703125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
@@ -928,7 +931,7 @@
       <c r="N1" s="6"/>
       <c r="O1" s="7"/>
     </row>
-    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>6</v>
       </c>
@@ -938,8 +941,12 @@
       <c r="C2" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="D2" s="11">
+        <v>43892</v>
+      </c>
+      <c r="E2" s="11">
+        <v>43953</v>
+      </c>
       <c r="F2" s="10">
         <v>43866</v>
       </c>
@@ -947,7 +954,7 @@
         <v>11</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="I2" s="13"/>
       <c r="J2" s="9"/>
@@ -957,7 +964,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
@@ -967,7 +974,7 @@
       <c r="C3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="49">
+      <c r="D3" s="46">
         <v>43865</v>
       </c>
       <c r="E3" s="1"/>
@@ -988,7 +995,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="21"/>
     </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>7</v>
       </c>
@@ -1017,7 +1024,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="21"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1053,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="21"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1082,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="21"/>
     </row>
-    <row r="7" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1111,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="21"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>40</v>
       </c>
@@ -1133,7 +1140,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="21"/>
     </row>
-    <row r="9" spans="1:15" s="35" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>39</v>
       </c>
@@ -1162,7 +1169,7 @@
       <c r="N9" s="39"/>
       <c r="O9" s="45"/>
     </row>
-    <row r="10" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>42</v>
       </c>
@@ -1189,7 +1196,7 @@
       <c r="N10" s="39"/>
       <c r="O10" s="45"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>16</v>
       </c>
@@ -1222,7 +1229,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="21"/>
     </row>
-    <row r="12" spans="1:15" ht="28" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
         <v>16</v>
       </c>
@@ -1253,7 +1260,7 @@
       <c r="N12" s="1"/>
       <c r="O12" s="21"/>
     </row>
-    <row r="13" spans="1:15" ht="28" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
         <v>16</v>
       </c>
@@ -1284,7 +1291,7 @@
       <c r="N13" s="1"/>
       <c r="O13" s="21"/>
     </row>
-    <row r="14" spans="1:15" ht="28" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>16</v>
       </c>
@@ -1315,7 +1322,7 @@
       <c r="N14" s="1"/>
       <c r="O14" s="21"/>
     </row>
-    <row r="15" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
         <v>16</v>
       </c>
@@ -1346,7 +1353,7 @@
       <c r="N15" s="1"/>
       <c r="O15" s="21"/>
     </row>
-    <row r="16" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
         <v>23</v>
       </c>
@@ -1377,7 +1384,7 @@
       <c r="N16" s="1"/>
       <c r="O16" s="21"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
         <v>24</v>
       </c>
@@ -1406,7 +1413,7 @@
       <c r="N17" s="1"/>
       <c r="O17" s="21"/>
     </row>
-    <row r="18" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>25</v>
       </c>
@@ -1435,17 +1442,17 @@
       <c r="N18" s="1"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="46" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
       <c r="I19" s="20"/>
       <c r="J19" s="25"/>
       <c r="K19" s="1"/>
@@ -1454,7 +1461,7 @@
       <c r="N19" s="1"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="29"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1471,7 +1478,7 @@
       <c r="N20" s="1"/>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="29"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1488,7 +1495,7 @@
       <c r="N21" s="1"/>
       <c r="O21" s="21"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1505,7 +1512,7 @@
       <c r="N22" s="1"/>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="29"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1522,7 +1529,7 @@
       <c r="N23" s="1"/>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="29"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1539,7 +1546,7 @@
       <c r="N24" s="1"/>
       <c r="O24" s="21"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="29"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1556,7 +1563,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="21"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="29"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1573,7 +1580,7 @@
       <c r="N26" s="1"/>
       <c r="O26" s="21"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="29"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1590,7 +1597,7 @@
       <c r="N27" s="1"/>
       <c r="O27" s="21"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1607,7 +1614,7 @@
       <c r="N28" s="1"/>
       <c r="O28" s="21"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1624,7 +1631,7 @@
       <c r="N29" s="1"/>
       <c r="O29" s="21"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1641,7 +1648,7 @@
       <c r="N30" s="1"/>
       <c r="O30" s="21"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1658,7 +1665,7 @@
       <c r="N31" s="1"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>

</xml_diff>

<commit_message>
updating that PWM searching is done Signed-off-by: marcellesamir <marcelle.samir.s@gmail.com>
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO.SXM1\Documents\GitHub\INMOOV_project\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\embedded\ITI\projects\side project\repo\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34FF992-D613-43D2-ADC2-D673E4BDAD40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E8F8A-92EC-4121-95F3-423135115A27}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="68" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Mina,Refaat</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -880,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1017,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="1"/>

</xml_diff>

<commit_message>
add new matlab script
</commit_message>
<xml_diff>
--- a/Project Plan/INMOOV-project-plan.xlsx
+++ b/Project Plan/INMOOV-project-plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\embedded\ITI\projects\side project\repo\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO.SXM1\Documents\GitHub\INMOOV_project\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6E8F8A-92EC-4121-95F3-423135115A27}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9D6C84-DB3A-4AC2-A86C-D0C402CD7386}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="68" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="46">
   <si>
     <t>Task</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>refaat,marcelle</t>
   </si>
 </sst>
 </file>
@@ -881,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +968,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
@@ -1009,7 +1012,9 @@
       <c r="D4" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="11">
+        <v>43984</v>
+      </c>
       <c r="F4" s="16">
         <v>43866</v>
       </c>
@@ -1017,7 +1022,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I4" s="19"/>
       <c r="J4" s="1"/>
@@ -1296,7 +1301,9 @@
       <c r="D13" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="22"/>
+      <c r="E13" s="22">
+        <v>43869</v>
+      </c>
       <c r="F13" s="22">
         <v>43864</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>17</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I13" s="30"/>
       <c r="J13" s="1"/>
@@ -1389,7 +1396,9 @@
       <c r="D16" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="22">
+        <v>43868</v>
+      </c>
       <c r="F16" s="22">
         <v>43866</v>
       </c>
@@ -1397,7 +1406,7 @@
         <v>14</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="I16" s="30"/>
       <c r="J16" s="1"/>
@@ -1480,7 +1489,7 @@
       <c r="F19" s="47"/>
       <c r="G19" s="47"/>
       <c r="H19" s="48"/>
-      <c r="I19" s="20"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="25"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1488,16 +1497,28 @@
       <c r="N19" s="1"/>
       <c r="O19" s="21"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="1"/>
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="38"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="16">
+        <v>43866</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="44"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1505,33 +1526,44 @@
       <c r="N20" s="1"/>
       <c r="O20" s="21"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="21"/>
+    <row r="21" spans="1:15" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="40">
+        <v>43865</v>
+      </c>
+      <c r="D21" s="38"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="16">
+        <v>43866</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="30"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="45"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="1"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="30"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1539,16 +1571,28 @@
       <c r="N22" s="1"/>
       <c r="O22" s="21"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="1"/>
+    <row r="23" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="38"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22">
+        <v>43866</v>
+      </c>
+      <c r="G23" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="30"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1556,15 +1600,27 @@
       <c r="N23" s="1"/>
       <c r="O23" s="21"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="18"/>
+    <row r="24" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="38"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22">
+        <v>43866</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1692,29 +1748,62 @@
       <c r="N31" s="1"/>
       <c r="O31" s="21"/>
     </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="34"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="27"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="28"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="29"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="21"/>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="29"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="21"/>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="34"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="27"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
+      <c r="N34" s="26"/>
+      <c r="O34" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A19:H19"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H20:H32 H2:H18" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H18 H20:H34" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Asseigned,In progress,done,Revised"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>